<commit_message>
solved problem 2 part a
</commit_message>
<xml_diff>
--- a/2020/data/problem_2_values.xlsx
+++ b/2020/data/problem_2_values.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyled\coding\advent_of_code\2020\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C518BE-B781-4D29-87A0-22FD1296BE21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840F0C9D-CA48-4F1F-B1B9-B61D51D53EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2115" windowWidth="21600" windowHeight="13485" xr2:uid="{49409D53-6B50-4E22-8E35-3F4A7A96D9B1}"/>
+    <workbookView xWindow="3120" yWindow="2115" windowWidth="21600" windowHeight="13485" activeTab="1" xr2:uid="{49409D53-6B50-4E22-8E35-3F4A7A96D9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="1004">
   <si>
     <t>17-19 p: pwpzpfbrcpppjppbmppp</t>
   </si>
@@ -3037,13 +3038,22 @@
   </si>
   <si>
     <t>Values</t>
+  </si>
+  <si>
+    <t>1-3 a: abcde</t>
+  </si>
+  <si>
+    <t>1-3 b: cdefg</t>
+  </si>
+  <si>
+    <t>2-9 c: ccccccccc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3056,13 +3066,25 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Source Code Pro"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0F0F23"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3077,9 +3099,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3398,8 +3426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1A0F73-B177-4D6E-9719-FBA8ECEA3C12}">
   <dimension ref="A1:A1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8416,4 +8444,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F063E1-276A-49EA-AA99-FD8DB033C011}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>